<commit_message>
timesheet and reformat directory
</commit_message>
<xml_diff>
--- a/admin/timesheets/timesheet_template.xlsx
+++ b/admin/timesheets/timesheet_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kailesuoo/Downloads/NASA-JPL-Capstone/admin/timesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6EECE0-9CC3-554C-8403-37F4F986B67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D377233D-CC95-394F-9BE9-2E58069BD236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,25 +569,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="10">
-        <v>45970</v>
+        <v>46048</v>
       </c>
       <c r="C5" s="10">
-        <v>45971</v>
+        <v>46049</v>
       </c>
       <c r="D5" s="10">
-        <v>45972</v>
+        <v>46050</v>
       </c>
       <c r="E5" s="10">
-        <v>45973</v>
+        <v>46051</v>
       </c>
       <c r="F5" s="10">
-        <v>45974</v>
+        <v>46052</v>
       </c>
       <c r="G5" s="10">
-        <v>45975</v>
+        <v>46053</v>
       </c>
       <c r="H5" s="11">
-        <v>45976</v>
+        <v>46054</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>5</v>

</xml_diff>